<commit_message>
TelegramNotifierApp.py added default names for the 1st and 2nd sheets
</commit_message>
<xml_diff>
--- a/ResultsReporter/dist/TelegramListToSend.xlsx
+++ b/ResultsReporter/dist/TelegramListToSend.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timeo\PycharmProjects\SilaMisli2025\V1\ResultsReporter\dist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2A5234-7F57-4CD5-B0B8-B879A41917C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA2E944-B571-4015-8D24-B48EB05EC9B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{E369EFA5-D418-4E1B-8455-2F634F4111DF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{E369EFA5-D418-4E1B-8455-2F634F4111DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
-    <sheet name="TeamPhone" sheetId="2" r:id="rId2"/>
+    <sheet name="Phones" sheetId="2" r:id="rId2"/>
     <sheet name="Description" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TeamPhone!$B$2:$B$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Phones!$B$2:$B$17</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>Phone Number</t>
   </si>
@@ -150,6 +150,10 @@
   </si>
   <si>
     <t>+1204….</t>
+  </si>
+  <si>
+    <t>If in an Excel file, there are many sheets, then set the sheets' names as here: 'Results'==&gt;'ResultsToSend' and 'Phones'==&gt;'TeamsPhones'. 
+It will guarantee that the expected data will be found accordingly.</t>
   </si>
 </sst>
 </file>
@@ -170,7 +174,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -201,6 +205,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -214,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -229,6 +239,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -891,8 +904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F089B8A8-54EB-4721-8A5A-7118779B8CC7}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1009,9 +1022,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC68490E-0B47-4FF3-B227-126B27B152ED}">
-  <dimension ref="D1:D3"/>
+  <dimension ref="D1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -1035,6 +1048,11 @@
         <v>33</v>
       </c>
     </row>
+    <row r="4" spans="4:4" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="D4" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>